<commit_message>
Ändrat text i #58 samt korrigerat namn på två andra fans
</commit_message>
<xml_diff>
--- a/fan-overview-swe.xlsx
+++ b/fan-overview-swe.xlsx
@@ -1141,7 +1141,7 @@
     <t xml:space="preserve">Två dolda Pung/Kong (en kan vara utlagda som Concealed Kong)</t>
   </si>
   <si>
-    <t xml:space="preserve">Double Pungs</t>
+    <t xml:space="preserve">Double Pung</t>
   </si>
   <si>
     <t xml:space="preserve">Samma valör av Pung/Kong men var sin färg</t>
@@ -1177,7 +1177,7 @@
     <t xml:space="preserve">Last Tile</t>
   </si>
   <si>
-    <t xml:space="preserve">Mahjong på fjärde (sista) synliga exemplaret av en bricka</t>
+    <t xml:space="preserve">Mahjong på sista exemplaret av en bricka, där alla övriga finns synliga bland slängda och/eller utlagda brickor</t>
   </si>
   <si>
     <t xml:space="preserve">Två utlagda Kongs. Får kombineras med Concealed Kong, Fan #67</t>
@@ -1735,7 +1735,7 @@
     <t xml:space="preserve">En dold hand med 1,1,1,2,3,4,5,6,7,8,9,9,9 i samma färg samt en till av dessa brickor</t>
   </si>
   <si>
-    <t xml:space="preserve">All Greens</t>
+    <t xml:space="preserve">All Green</t>
   </si>
   <si>
     <t xml:space="preserve">En hand endast bestående av brickorna 2,3,4,6,8 i bambu och/eller gröna drakar</t>
@@ -1753,7 +1753,7 @@
     <t xml:space="preserve">Pungs/Kongs i alla fyra vindar</t>
   </si>
   <si>
-    <t xml:space="preserve">Release 1.6 2024-02-01, CC BY-SA 4.0
+    <t xml:space="preserve">Release 1.7 2024-02-02, CC BY-SA 4.0
 Ladda ner senaste version från https://github.com/dstahlberg/mahjong
 Synpunkter/kommentarer/fel, maila gärna mahjongihaninge@gmail.com
 Baserat på Mahjong Competition Rules, Second Edition, December 2014, WMO - World Mahjong Organisation</t>
@@ -2655,8 +2655,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="11.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3765,7 +3765,7 @@
       <c r="B83" s="24"/>
       <c r="AMJ83" s="0"/>
     </row>
-    <row r="84" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="36" t="s">
         <v>212</v>
       </c>

</xml_diff>

<commit_message>
Clarification of rules for Kongs #5,17,57
</commit_message>
<xml_diff>
--- a/fan-overview-swe.xlsx
+++ b/fan-overview-swe.xlsx
@@ -1132,7 +1132,7 @@
     <t xml:space="preserve">En hand utan ettor, nior, vindar eller drakar</t>
   </si>
   <si>
-    <t xml:space="preserve">En utlagd dold Kong byggd på dragen bricka</t>
+    <t xml:space="preserve">En dold Kong, byggd på brickor dragna från muren</t>
   </si>
   <si>
     <t xml:space="preserve">Two Concealed Pungs</t>
@@ -1144,7 +1144,7 @@
     <t xml:space="preserve">Double Pung</t>
   </si>
   <si>
-    <t xml:space="preserve">Samma valör av Pung/Kong men var sin färg</t>
+    <t xml:space="preserve">Samma valör av Pung/Kong men i var sin färg</t>
   </si>
   <si>
     <t xml:space="preserve">En hand med alla fyra exemplar av en bricka, där de inte använts i en Kong</t>
@@ -1180,7 +1180,7 @@
     <t xml:space="preserve">Mahjong på sista exemplaret av en bricka, där alla övriga finns synliga bland slängda och/eller utlagda brickor</t>
   </si>
   <si>
-    <t xml:space="preserve">Två utlagda Kongs. Får kombineras med Concealed Kong, Fan #67</t>
+    <t xml:space="preserve">Två Kongs, byggda av slängda brickor eller dolda.  En kan kombineras med Concealed Kong, Fan #67</t>
   </si>
   <si>
     <t xml:space="preserve">Fully Concealed Hand</t>
@@ -1195,7 +1195,7 @@
     <t xml:space="preserve">Två Pungs/Kongs i drakar </t>
   </si>
   <si>
-    <t xml:space="preserve">Fyra utlagda kombinationer och Mahjong på slängd bricka</t>
+    <t xml:space="preserve">Fyra utlagda kombinationer byggda av slängda brickor och Mahjong på slängd bricka</t>
   </si>
   <si>
     <t xml:space="preserve">All Types</t>
@@ -1426,7 +1426,7 @@
     <t xml:space="preserve">Reversible Tiles</t>
   </si>
   <si>
-    <t xml:space="preserve">Endast brickor som ser likadana ut vända upp och ner; Cirkel 1,2,3,4,5,8,9, Bambu 2,4,5,6,8,9 och vit drake</t>
+    <t xml:space="preserve">En hand där alla kombinationer består av brickor som ser likadana ut vända upp och ner</t>
   </si>
   <si>
     <t xml:space="preserve">Mixed Straight</t>
@@ -1660,7 +1660,7 @@
     <t xml:space="preserve">Alla kombinationer (Pungs, Kongs, Par) består av ettor, nior, vindar eller drakar</t>
   </si>
   <si>
-    <t xml:space="preserve">Tre Kongs, utlagda eller på hand</t>
+    <t xml:space="preserve">Tre Kongs, byggda av slängda brickor eller dolda.  Får kombineras med Concealed Kong, Fan #67</t>
   </si>
   <si>
     <t xml:space="preserve">Four Pure Shifted Chows</t>
@@ -1726,7 +1726,7 @@
     <t xml:space="preserve">En hand bestående av sju par i samma färg i följd, Ex 1-1, 2-2, 3-3, 4-4 osv</t>
   </si>
   <si>
-    <t xml:space="preserve">En hand med fyra Kongs</t>
+    <t xml:space="preserve">Fyra Kongs, byggda av slängda brickor eller dolda.  Får kombineras med Concealed Kong, Fan #67</t>
   </si>
   <si>
     <t xml:space="preserve">Nine Gates</t>
@@ -1738,7 +1738,7 @@
     <t xml:space="preserve">All Green</t>
   </si>
   <si>
-    <t xml:space="preserve">En hand endast bestående av brickorna 2,3,4,6,8 i bambu och/eller gröna drakar</t>
+    <t xml:space="preserve">En hand där alla kombinationer består av brickorna 2,3,4,6,8 i bambu och/eller gröna drakar</t>
   </si>
   <si>
     <t xml:space="preserve">Big Three Dragons</t>
@@ -1753,10 +1753,26 @@
     <t xml:space="preserve">Pungs/Kongs i alla fyra vindar</t>
   </si>
   <si>
-    <t xml:space="preserve">Release 1.7 2024-02-02, CC BY-SA 4.0
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="6"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Release 1.9 2024-02-16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, CC BY-SA 4.0
 Ladda ner senaste version från https://github.com/dstahlberg/mahjong
 Synpunkter/kommentarer/fel, maila gärna mahjongihaninge@gmail.com
 Baserat på Mahjong Competition Rules, Second Edition, December 2014, WMO - World Mahjong Organisation</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2112,7 +2128,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2653,10 +2669,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ84"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="11.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3773,6 +3789,7 @@
       <c r="C84" s="36"/>
       <c r="D84" s="36"/>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A84:D84"/>

</xml_diff>